<commit_message>
Updated the location in excel
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spand\eclipse-workspace19\FTS_Automation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SPenumetcha\git\FTS-Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F40535-C7E9-434E-9E5F-5ECA8E3A18F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF19C3D-6578-4479-ACAA-DD13D6EBF2A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{27D9C0EC-8EEA-4AA9-BF2F-B4194E1BD2E7}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="FilesToUpload" sheetId="4" r:id="rId2"/>
     <sheet name="FIles to upload" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" calcOnSave="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="56">
   <si>
     <t>005010X222A1</t>
   </si>
@@ -143,71 +143,65 @@
     <t>Env</t>
   </si>
   <si>
-    <t>Ehsquincyst21!!</t>
-  </si>
-  <si>
-    <t>Ehsquincyst23!!</t>
-  </si>
-  <si>
-    <t>ginc_FileName</t>
-  </si>
-  <si>
-    <t>GINCPROFTXT</t>
-  </si>
-  <si>
-    <t>GINCINSTTXT</t>
-  </si>
-  <si>
-    <t>837PX12_TCP1302_Gosnold_Inc</t>
-  </si>
-  <si>
-    <t>ginc_FileType</t>
-  </si>
-  <si>
-    <t>gatra_FileName</t>
-  </si>
-  <si>
-    <t>gatra_FileType</t>
-  </si>
-  <si>
-    <t>DKGATRAHIPAA837P01</t>
-  </si>
-  <si>
-    <t>bmc_FileName</t>
-  </si>
-  <si>
-    <t>bmc_FileType</t>
-  </si>
-  <si>
-    <t>DKOXIINST02</t>
-  </si>
-  <si>
-    <t>DKOXIINST05</t>
-  </si>
-  <si>
     <t>User</t>
   </si>
   <si>
-    <t>bmc</t>
-  </si>
-  <si>
     <t>Files</t>
   </si>
   <si>
-    <t>C:\Users\spand\eclipse-workspace19\FTS_Automation\FTS\GINC - PROF and INST</t>
-  </si>
-  <si>
-    <t>C:\Users\spand\eclipse-workspace19\FTS_Automation\FTS\BMC</t>
-  </si>
-  <si>
-    <t>C:\Users\spand\eclipse-workspace19\FTS_Automation\FTS\GATRA - PROF</t>
+    <t>LargeFileSpectrum.HIPAA837P</t>
+  </si>
+  <si>
+    <t>LARGEBPC.HIPAA937P</t>
+  </si>
+  <si>
+    <t>bphc_FileType</t>
+  </si>
+  <si>
+    <t>bphc_FileName</t>
+  </si>
+  <si>
+    <t>hpoint_FileType</t>
+  </si>
+  <si>
+    <t>hpoint_FileName</t>
+  </si>
+  <si>
+    <t>sinc1_FileName</t>
+  </si>
+  <si>
+    <t>sinc1_FileType</t>
+  </si>
+  <si>
+    <t>sinc1</t>
+  </si>
+  <si>
+    <t>EhsBostonQA22!!</t>
+  </si>
+  <si>
+    <t>bphc</t>
+  </si>
+  <si>
+    <t>hpoint</t>
+  </si>
+  <si>
+    <t>LargeHighPointTreatCtr.HIPAA837I</t>
+  </si>
+  <si>
+    <t>\\ehs-clu-bos-001.ehs.govt.state.ma.us\File Services\QA\Projects\VG\FTS Automation\Diane - test files\Original</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>High Point Treatment Ctr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,6 +213,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -307,8 +309,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -349,12 +352,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -667,282 +669,163 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22251FF1-831B-45EE-AE4B-F0D232E69A17}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="15.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="70" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="95.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" s="21" t="s">
+      <c r="D1" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="20" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" s="20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="19" t="s">
-        <v>11</v>
+      <c r="B2" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="19" t="s">
+      <c r="B4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>56</v>
-      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{9D00739F-BBF4-473B-8079-00F17CBF20A7}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{14F7A31A-0FEA-43D6-8CA6-F6D70731920E}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{369A816C-2064-4495-B878-3CC27F317B95}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8126D4D5-8330-4D4A-BB7E-4AAF888AAFAA}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.36328125" customWidth="1"/>
-    <col min="4" max="4" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.08984375" customWidth="1"/>
+    <col min="3" max="3" width="34.36328125" customWidth="1"/>
+    <col min="4" max="4" width="17.1796875" customWidth="1"/>
+    <col min="5" max="5" width="34.1796875" customWidth="1"/>
     <col min="6" max="6" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B1" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="15" t="s">
         <v>44</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="7" t="s">
+      <c r="C2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="E2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>1</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -955,7 +838,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2086FBD-C84A-4E68-88D0-A0691E40A11C}">
   <dimension ref="B2:E29"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24:C29"/>
     </sheetView>
   </sheetViews>

</xml_diff>